<commit_message>
replace HBET:3,5 with HBET:3-5 in Romania source data and mapping scheme
</commit_message>
<xml_diff>
--- a/res_exposure_source_data/data_Romania_RES_census-buildings_mapping.xlsx
+++ b/res_exposure_source_data/data_Romania_RES_census-buildings_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helencrowley/Documents/5-GitHub/esrm20_exposure/res_exposure_source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7E66DD-CF24-9D4E-ADE4-B26403ABE453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2691E58C-6140-B544-80F2-F4E5697C00D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5800" yWindow="980" windowWidth="26840" windowHeight="15220" xr2:uid="{C812A46A-F076-D84F-9A3A-6DA32F506C74}"/>
+    <workbookView xWindow="10420" yWindow="680" windowWidth="26840" windowHeight="15220" xr2:uid="{C812A46A-F076-D84F-9A3A-6DA32F506C74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="314">
   <si>
     <t>CR+CIP/LFINF+CDN/H:1/YPRE:1945</t>
   </si>
@@ -720,9 +720,6 @@
     <t>CR+CIP/LFINF+CDH/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFINF+CDH/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFINF+CDH/HBET:6-</t>
   </si>
   <si>
@@ -732,27 +729,18 @@
     <t>CR+CIP/LFINF+CDL/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFINF+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFINF+CDM/H:1</t>
   </si>
   <si>
     <t>CR+CIP/LFINF+CDM/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFINF+CDM/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFINF+CDM/HBET:6-</t>
   </si>
   <si>
     <t>CR+CIP/LFINF+CDN/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFINF+CDN/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFINF+CDN/HBET:6-</t>
   </si>
   <si>
@@ -762,9 +750,6 @@
     <t>CR+CIP/LFM+CDH/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFM+CDH/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFM+CDH/HBET:6-</t>
   </si>
   <si>
@@ -774,9 +759,6 @@
     <t>CR+CIP/LFM+CDL/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFM+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFM+CDL/HBET:6-</t>
   </si>
   <si>
@@ -786,9 +768,6 @@
     <t>CR+CIP/LFM+CDM/H:2</t>
   </si>
   <si>
-    <t>CR+CIP/LFM+CDM/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+CIP/LFM+CDM/HBET:6-</t>
   </si>
   <si>
@@ -798,27 +777,18 @@
     <t>CR+PC/LFM+CDL/H:2</t>
   </si>
   <si>
-    <t>CR+PC/LFM+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+PC/LFM+CDL/HBET:6-</t>
   </si>
   <si>
     <t>CR+PC/LWAL+CDL/H:2</t>
   </si>
   <si>
-    <t>CR+PC/LWAL+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+PC/LWAL+CDL/HBET:6-</t>
   </si>
   <si>
     <t>CR+PC/LWAL+CDM/H:2</t>
   </si>
   <si>
-    <t>CR+PC/LWAL+CDM/HBET:3,5</t>
-  </si>
-  <si>
     <t>CR+PC/LWAL+CDM/HBET:6-</t>
   </si>
   <si>
@@ -828,9 +798,6 @@
     <t>MCF/LWAL+CDH/H:2</t>
   </si>
   <si>
-    <t>MCF/LWAL+CDH/HBET:3,5</t>
-  </si>
-  <si>
     <t>MCF/LWAL+CDH/HBET:6-</t>
   </si>
   <si>
@@ -840,9 +807,6 @@
     <t>MCF/LWAL+CDL/H:2</t>
   </si>
   <si>
-    <t>MCF/LWAL+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>MCF/LWAL+CDL/HBET:6-</t>
   </si>
   <si>
@@ -864,9 +828,6 @@
     <t>MCF/LWAL+CDN/HBET:6-</t>
   </si>
   <si>
-    <t>MCF/LWAL+CDN/HBET:3,5</t>
-  </si>
-  <si>
     <t>MCF/LWAL+CDN/H:2</t>
   </si>
   <si>
@@ -876,9 +837,6 @@
     <t>MUR/LWAL+CDN/H:2</t>
   </si>
   <si>
-    <t>MUR/LWAL+CDN/HBET:3,5</t>
-  </si>
-  <si>
     <t>MUR/LWAL+CDN/HBET:6-</t>
   </si>
   <si>
@@ -891,18 +849,12 @@
     <t>W/LFM+CDL/H:1</t>
   </si>
   <si>
-    <t>W/LFM+CDH/HBET:3,5</t>
-  </si>
-  <si>
     <t>W/LFM+CDH/HBET:6-</t>
   </si>
   <si>
     <t>W/LFM+CDL/H:2</t>
   </si>
   <si>
-    <t>W/LFM+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>W/LFM+CDL/HBET:6-</t>
   </si>
   <si>
@@ -912,9 +864,6 @@
     <t>W/LFM+CDM/H:2</t>
   </si>
   <si>
-    <t>W/LFM+CDM/HBET:3,5</t>
-  </si>
-  <si>
     <t>W/LFM+CDM/HBET:6-</t>
   </si>
   <si>
@@ -924,15 +873,9 @@
     <t>W/LFM+CDN/H:2</t>
   </si>
   <si>
-    <t>W/LFM+CDN/HBET:3,5</t>
-  </si>
-  <si>
     <t>W/LFM+CDN/HBET:6-</t>
   </si>
   <si>
-    <t>MCF/LWAL+CDM/HBET:3,5</t>
-  </si>
-  <si>
     <t>MUR/LWAL+CDL/H:1</t>
   </si>
   <si>
@@ -945,15 +888,9 @@
     <t>MUR+ADO/LWAL+CDN/H:2</t>
   </si>
   <si>
-    <t>MUR+ADO/LWAL+CDN/HBET:3,5</t>
-  </si>
-  <si>
     <t>MUR+ADO/LWAL+CDN/HBET:6-</t>
   </si>
   <si>
-    <t>MUR/LWAL+CDL/HBET:3,5</t>
-  </si>
-  <si>
     <t>MUR/LWAL+CDL/HBET:6-</t>
   </si>
   <si>
@@ -961,6 +898,78 @@
   </si>
   <si>
     <t xml:space="preserve">Mapped_typology </t>
+  </si>
+  <si>
+    <t>CR+CIP/LFINF+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFINF+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFINF+CDM/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFINF+CDN/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFM+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFM+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFM+CDM/HBET:3-5/YBET:1977-1992</t>
+  </si>
+  <si>
+    <t>CR+CIP/LFM+CDM/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+PC/LDUAL+CDM/HBET:3-5/YBET:1977-1992</t>
+  </si>
+  <si>
+    <t>CR+PC/LFM+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+PC/LFM+CDM/HBET:3-5/YBET:1977-1992</t>
+  </si>
+  <si>
+    <t>CR+PC/LWAL+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>CR+PC/LWAL+CDM/HBET:3-5/YBET:1977-1992</t>
+  </si>
+  <si>
+    <t>CR+PC/LWAL+CDM/HBET:3-5</t>
+  </si>
+  <si>
+    <t>MUR+ADO/LWAL+CDN/HBET:3-5</t>
+  </si>
+  <si>
+    <t>MUR/LWAL+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>MCF/LWAL+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>MCF/LWAL+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>MCF/LWAL+CDN/HBET:3-5</t>
+  </si>
+  <si>
+    <t>MUR/LWAL+CDN/HBET:3-5</t>
+  </si>
+  <si>
+    <t>W/LFM+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>W/LFM+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>W/LFM+CDM/HBET:3-5</t>
+  </si>
+  <si>
+    <t>W/LFM+CDN/HBET:3-5</t>
   </si>
 </sst>
 </file>
@@ -1323,21 +1332,22 @@
   <dimension ref="A1:B227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" customWidth="1"/>
     <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="B1" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1377,7 +1387,7 @@
         <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1385,7 +1395,7 @@
         <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>230</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1393,7 +1403,7 @@
         <v>182</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1401,7 +1411,7 @@
         <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1409,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1417,7 +1427,7 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1425,7 +1435,7 @@
         <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1433,7 +1443,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1441,7 +1451,7 @@
         <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1449,7 +1459,7 @@
         <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1457,7 +1467,7 @@
         <v>179</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1481,7 +1491,7 @@
         <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1489,7 +1499,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1497,7 +1507,7 @@
         <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>240</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1505,7 +1515,7 @@
         <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>240</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1513,7 +1523,7 @@
         <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1521,7 +1531,7 @@
         <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1529,7 +1539,7 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1537,7 +1547,7 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1545,7 +1555,7 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1553,7 +1563,7 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1561,7 +1571,7 @@
         <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1569,7 +1579,7 @@
         <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1577,7 +1587,7 @@
         <v>181</v>
       </c>
       <c r="B31" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1585,7 +1595,7 @@
         <v>183</v>
       </c>
       <c r="B32" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -1593,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1601,7 +1611,7 @@
         <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1609,7 +1619,7 @@
         <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>248</v>
+        <v>295</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1617,7 +1627,7 @@
         <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1633,7 +1643,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1649,7 +1659,7 @@
         <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1657,7 +1667,7 @@
         <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1665,7 +1675,7 @@
         <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -1673,7 +1683,7 @@
         <v>178</v>
       </c>
       <c r="B43" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1697,7 +1707,7 @@
         <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>298</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1713,7 +1723,7 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1721,7 +1731,7 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1729,7 +1739,7 @@
         <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>256</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1737,7 +1747,7 @@
         <v>173</v>
       </c>
       <c r="B51" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1761,7 +1771,7 @@
         <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1785,7 +1795,7 @@
         <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1793,7 +1803,7 @@
         <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>259</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1801,7 +1811,7 @@
         <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1833,7 +1843,7 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1841,7 +1851,7 @@
         <v>122</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>302</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1849,7 +1859,7 @@
         <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>262</v>
+        <v>303</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1865,7 +1875,7 @@
         <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1873,7 +1883,7 @@
         <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1881,7 +1891,7 @@
         <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1889,7 +1899,7 @@
         <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -1897,7 +1907,7 @@
         <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1905,7 +1915,7 @@
         <v>98</v>
       </c>
       <c r="B72" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1913,7 +1923,7 @@
         <v>100</v>
       </c>
       <c r="B73" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1921,7 +1931,7 @@
         <v>102</v>
       </c>
       <c r="B74" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1929,7 +1939,7 @@
         <v>96</v>
       </c>
       <c r="B75" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1937,7 +1947,7 @@
         <v>154</v>
       </c>
       <c r="B76" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1945,7 +1955,7 @@
         <v>156</v>
       </c>
       <c r="B77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1953,7 +1963,7 @@
         <v>158</v>
       </c>
       <c r="B78" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1961,7 +1971,7 @@
         <v>152</v>
       </c>
       <c r="B79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1969,7 +1979,7 @@
         <v>209</v>
       </c>
       <c r="B80" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1977,7 +1987,7 @@
         <v>211</v>
       </c>
       <c r="B81" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1985,7 +1995,7 @@
         <v>213</v>
       </c>
       <c r="B82" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1993,7 +2003,7 @@
         <v>207</v>
       </c>
       <c r="B83" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -2001,7 +2011,7 @@
         <v>56</v>
       </c>
       <c r="B84" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -2009,7 +2019,7 @@
         <v>113</v>
       </c>
       <c r="B85" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -2017,7 +2027,7 @@
         <v>169</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -2025,7 +2035,7 @@
         <v>224</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -2033,7 +2043,7 @@
         <v>54</v>
       </c>
       <c r="B88" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -2041,7 +2051,7 @@
         <v>55</v>
       </c>
       <c r="B89" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -2049,7 +2059,7 @@
         <v>111</v>
       </c>
       <c r="B90" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -2057,7 +2067,7 @@
         <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -2065,7 +2075,7 @@
         <v>166</v>
       </c>
       <c r="B92" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -2073,7 +2083,7 @@
         <v>167</v>
       </c>
       <c r="B93" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -2081,7 +2091,7 @@
         <v>168</v>
       </c>
       <c r="B94" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -2089,7 +2099,7 @@
         <v>222</v>
       </c>
       <c r="B95" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -2097,7 +2107,7 @@
         <v>223</v>
       </c>
       <c r="B96" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -2105,7 +2115,7 @@
         <v>51</v>
       </c>
       <c r="B97" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -2113,7 +2123,7 @@
         <v>108</v>
       </c>
       <c r="B98" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -2121,7 +2131,7 @@
         <v>164</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -2129,7 +2139,7 @@
         <v>219</v>
       </c>
       <c r="B100" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -2137,7 +2147,7 @@
         <v>52</v>
       </c>
       <c r="B101" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -2145,7 +2155,7 @@
         <v>53</v>
       </c>
       <c r="B102" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -2153,7 +2163,7 @@
         <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -2161,7 +2171,7 @@
         <v>110</v>
       </c>
       <c r="B104" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -2169,7 +2179,7 @@
         <v>165</v>
       </c>
       <c r="B105" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -2177,7 +2187,7 @@
         <v>220</v>
       </c>
       <c r="B106" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -2185,7 +2195,7 @@
         <v>221</v>
       </c>
       <c r="B107" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -2193,7 +2203,7 @@
         <v>50</v>
       </c>
       <c r="B108" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -2201,7 +2211,7 @@
         <v>49</v>
       </c>
       <c r="B109" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -2209,7 +2219,7 @@
         <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -2217,7 +2227,7 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -2225,7 +2235,7 @@
         <v>163</v>
       </c>
       <c r="B112" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -2233,7 +2243,7 @@
         <v>162</v>
       </c>
       <c r="B113" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2241,7 +2251,7 @@
         <v>218</v>
       </c>
       <c r="B114" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -2249,7 +2259,7 @@
         <v>217</v>
       </c>
       <c r="B115" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
@@ -2257,7 +2267,7 @@
         <v>44</v>
       </c>
       <c r="B116" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -2265,7 +2275,7 @@
         <v>46</v>
       </c>
       <c r="B117" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -2273,7 +2283,7 @@
         <v>101</v>
       </c>
       <c r="B118" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -2281,7 +2291,7 @@
         <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
@@ -2289,7 +2299,7 @@
         <v>212</v>
       </c>
       <c r="B120" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -2297,7 +2307,7 @@
         <v>157</v>
       </c>
       <c r="B121" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -2305,7 +2315,7 @@
         <v>159</v>
       </c>
       <c r="B122" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -2313,7 +2323,7 @@
         <v>214</v>
       </c>
       <c r="B123" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -2321,7 +2331,7 @@
         <v>22</v>
       </c>
       <c r="B124" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -2329,7 +2339,7 @@
         <v>29</v>
       </c>
       <c r="B125" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -2337,7 +2347,7 @@
         <v>23</v>
       </c>
       <c r="B126" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -2345,7 +2355,7 @@
         <v>30</v>
       </c>
       <c r="B127" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
@@ -2353,7 +2363,7 @@
         <v>79</v>
       </c>
       <c r="B128" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
@@ -2361,7 +2371,7 @@
         <v>86</v>
       </c>
       <c r="B129" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -2369,7 +2379,7 @@
         <v>80</v>
       </c>
       <c r="B130" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -2377,7 +2387,7 @@
         <v>87</v>
       </c>
       <c r="B131" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -2385,7 +2395,7 @@
         <v>136</v>
       </c>
       <c r="B132" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -2393,7 +2403,7 @@
         <v>143</v>
       </c>
       <c r="B133" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -2401,7 +2411,7 @@
         <v>137</v>
       </c>
       <c r="B134" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -2409,7 +2419,7 @@
         <v>144</v>
       </c>
       <c r="B135" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -2417,7 +2427,7 @@
         <v>190</v>
       </c>
       <c r="B136" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -2425,7 +2435,7 @@
         <v>197</v>
       </c>
       <c r="B137" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -2433,7 +2443,7 @@
         <v>191</v>
       </c>
       <c r="B138" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -2441,7 +2451,7 @@
         <v>198</v>
       </c>
       <c r="B139" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -2449,7 +2459,7 @@
         <v>142</v>
       </c>
       <c r="B140" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
@@ -2457,7 +2467,7 @@
         <v>20</v>
       </c>
       <c r="B141" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -2465,7 +2475,7 @@
         <v>27</v>
       </c>
       <c r="B142" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -2473,7 +2483,7 @@
         <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -2481,7 +2491,7 @@
         <v>28</v>
       </c>
       <c r="B144" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -2489,7 +2499,7 @@
         <v>77</v>
       </c>
       <c r="B145" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
@@ -2497,7 +2507,7 @@
         <v>84</v>
       </c>
       <c r="B146" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
@@ -2505,7 +2515,7 @@
         <v>78</v>
       </c>
       <c r="B147" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
@@ -2513,7 +2523,7 @@
         <v>85</v>
       </c>
       <c r="B148" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
@@ -2521,7 +2531,7 @@
         <v>134</v>
       </c>
       <c r="B149" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
@@ -2529,7 +2539,7 @@
         <v>141</v>
       </c>
       <c r="B150" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
@@ -2537,7 +2547,7 @@
         <v>135</v>
       </c>
       <c r="B151" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
@@ -2545,7 +2555,7 @@
         <v>188</v>
       </c>
       <c r="B152" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -2553,7 +2563,7 @@
         <v>195</v>
       </c>
       <c r="B153" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
@@ -2561,7 +2571,7 @@
         <v>189</v>
       </c>
       <c r="B154" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
@@ -2569,7 +2579,7 @@
         <v>196</v>
       </c>
       <c r="B155" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -2577,7 +2587,7 @@
         <v>47</v>
       </c>
       <c r="B156" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -2585,7 +2595,7 @@
         <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
@@ -2593,7 +2603,7 @@
         <v>104</v>
       </c>
       <c r="B158" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
@@ -2601,7 +2611,7 @@
         <v>105</v>
       </c>
       <c r="B159" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
@@ -2609,7 +2619,7 @@
         <v>160</v>
       </c>
       <c r="B160" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
@@ -2617,7 +2627,7 @@
         <v>161</v>
       </c>
       <c r="B161" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
@@ -2625,7 +2635,7 @@
         <v>215</v>
       </c>
       <c r="B162" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
@@ -2633,7 +2643,7 @@
         <v>216</v>
       </c>
       <c r="B163" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
@@ -2641,7 +2651,7 @@
         <v>19</v>
       </c>
       <c r="B164" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
@@ -2649,7 +2659,7 @@
         <v>26</v>
       </c>
       <c r="B165" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
@@ -2657,7 +2667,7 @@
         <v>76</v>
       </c>
       <c r="B166" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
@@ -2665,7 +2675,7 @@
         <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
@@ -2673,7 +2683,7 @@
         <v>133</v>
       </c>
       <c r="B168" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -2681,7 +2691,7 @@
         <v>140</v>
       </c>
       <c r="B169" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
@@ -2689,7 +2699,7 @@
         <v>187</v>
       </c>
       <c r="B170" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
@@ -2697,7 +2707,7 @@
         <v>194</v>
       </c>
       <c r="B171" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
@@ -2705,7 +2715,7 @@
         <v>18</v>
       </c>
       <c r="B172" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
@@ -2713,7 +2723,7 @@
         <v>25</v>
       </c>
       <c r="B173" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
@@ -2721,7 +2731,7 @@
         <v>17</v>
       </c>
       <c r="B174" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
@@ -2729,7 +2739,7 @@
         <v>24</v>
       </c>
       <c r="B175" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
@@ -2737,7 +2747,7 @@
         <v>75</v>
       </c>
       <c r="B176" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
@@ -2745,7 +2755,7 @@
         <v>82</v>
       </c>
       <c r="B177" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
@@ -2753,7 +2763,7 @@
         <v>74</v>
       </c>
       <c r="B178" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
@@ -2761,7 +2771,7 @@
         <v>81</v>
       </c>
       <c r="B179" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
@@ -2769,7 +2779,7 @@
         <v>132</v>
       </c>
       <c r="B180" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
@@ -2777,7 +2787,7 @@
         <v>139</v>
       </c>
       <c r="B181" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
@@ -2785,7 +2795,7 @@
         <v>131</v>
       </c>
       <c r="B182" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
@@ -2793,7 +2803,7 @@
         <v>138</v>
       </c>
       <c r="B183" t="s">
-        <v>278</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
@@ -2801,7 +2811,7 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
@@ -2809,7 +2819,7 @@
         <v>193</v>
       </c>
       <c r="B185" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
@@ -2817,7 +2827,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
@@ -2825,7 +2835,7 @@
         <v>192</v>
       </c>
       <c r="B187" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
@@ -2833,7 +2843,7 @@
         <v>40</v>
       </c>
       <c r="B188" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
@@ -2841,7 +2851,7 @@
         <v>42</v>
       </c>
       <c r="B189" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
@@ -2849,7 +2859,7 @@
         <v>38</v>
       </c>
       <c r="B190" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
@@ -2857,7 +2867,7 @@
         <v>97</v>
       </c>
       <c r="B191" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
@@ -2865,7 +2875,7 @@
         <v>99</v>
       </c>
       <c r="B192" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
@@ -2873,7 +2883,7 @@
         <v>95</v>
       </c>
       <c r="B193" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
@@ -2881,7 +2891,7 @@
         <v>153</v>
       </c>
       <c r="B194" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
@@ -2889,7 +2899,7 @@
         <v>155</v>
       </c>
       <c r="B195" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
@@ -2897,7 +2907,7 @@
         <v>151</v>
       </c>
       <c r="B196" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
@@ -2905,7 +2915,7 @@
         <v>208</v>
       </c>
       <c r="B197" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
@@ -2913,7 +2923,7 @@
         <v>210</v>
       </c>
       <c r="B198" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
@@ -2921,7 +2931,7 @@
         <v>206</v>
       </c>
       <c r="B199" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
@@ -2929,7 +2939,7 @@
         <v>36</v>
       </c>
       <c r="B200" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
@@ -2937,7 +2947,7 @@
         <v>37</v>
       </c>
       <c r="B201" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
@@ -2945,7 +2955,7 @@
         <v>93</v>
       </c>
       <c r="B202" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
@@ -2953,7 +2963,7 @@
         <v>94</v>
       </c>
       <c r="B203" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
@@ -2961,7 +2971,7 @@
         <v>149</v>
       </c>
       <c r="B204" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
@@ -2969,7 +2979,7 @@
         <v>150</v>
       </c>
       <c r="B205" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
@@ -2977,7 +2987,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
@@ -2985,7 +2995,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
@@ -2993,7 +3003,7 @@
         <v>31</v>
       </c>
       <c r="B208" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
@@ -3001,7 +3011,7 @@
         <v>33</v>
       </c>
       <c r="B209" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
@@ -3009,7 +3019,7 @@
         <v>90</v>
       </c>
       <c r="B210" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
@@ -3017,7 +3027,7 @@
         <v>146</v>
       </c>
       <c r="B211" t="s">
-        <v>290</v>
+        <v>311</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
@@ -3025,7 +3035,7 @@
         <v>201</v>
       </c>
       <c r="B212" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
@@ -3033,7 +3043,7 @@
         <v>34</v>
       </c>
       <c r="B213" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
@@ -3041,7 +3051,7 @@
         <v>35</v>
       </c>
       <c r="B214" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
@@ -3049,7 +3059,7 @@
         <v>91</v>
       </c>
       <c r="B215" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
@@ -3057,7 +3067,7 @@
         <v>92</v>
       </c>
       <c r="B216" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
@@ -3065,7 +3075,7 @@
         <v>147</v>
       </c>
       <c r="B217" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
@@ -3073,7 +3083,7 @@
         <v>148</v>
       </c>
       <c r="B218" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
@@ -3081,7 +3091,7 @@
         <v>202</v>
       </c>
       <c r="B219" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
@@ -3089,7 +3099,7 @@
         <v>203</v>
       </c>
       <c r="B220" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
@@ -3097,7 +3107,7 @@
         <v>32</v>
       </c>
       <c r="B221" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
@@ -3105,7 +3115,7 @@
         <v>89</v>
       </c>
       <c r="B222" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
@@ -3113,7 +3123,7 @@
         <v>145</v>
       </c>
       <c r="B223" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
@@ -3121,7 +3131,7 @@
         <v>200</v>
       </c>
       <c r="B224" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
@@ -3129,7 +3139,7 @@
         <v>199</v>
       </c>
       <c r="B225" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
@@ -3137,7 +3147,7 @@
         <v>88</v>
       </c>
       <c r="B226" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
@@ -3145,7 +3155,7 @@
         <v>88</v>
       </c>
       <c r="B227" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>